<commit_message>
Minor Changes - Variable name changes
</commit_message>
<xml_diff>
--- a/data/Availability_List.xlsx
+++ b/data/Availability_List.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB99C740-E9AD-A448-9B31-97C0AA0DEF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9463E071-A9A8-A948-8A47-5A4C10F6FA76}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{F62BC5F4-B048-914E-9901-A2032154BA9D}"/>
+    <workbookView windowHeight="16440" windowWidth="27240" xWindow="12380" xr2:uid="{F62BC5F4-B048-914E-9901-A2032154BA9D}" yWindow="2800"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -60,12 +60,24 @@
   </si>
   <si>
     <t>AVAILABLE</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>12:00 PM</t>
+  </si>
+  <si>
+    <t>BUSY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/MM/yy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -116,19 +128,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -145,10 +158,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -183,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -235,7 +248,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -346,21 +359,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -377,7 +390,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -449,25 +462,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C808D-9F34-F242-8D47-07932BD88B7B}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C808D-9F34-F242-8D47-07932BD88B7B}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="A5" sqref="A5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="31.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -538,7 +551,24 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n" s="4">
+        <v>45593.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed: - Set Availability - Added new application outcome excel file - Able to add new application outcome - Changed doctor folder
</commit_message>
<xml_diff>
--- a/data/Availability_List.xlsx
+++ b/data/Availability_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9463E071-A9A8-A948-8A47-5A4C10F6FA76}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8C638F2F-B9D9-1942-9E61-D20222377F6A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="16440" windowWidth="27240" xWindow="12380" xr2:uid="{F62BC5F4-B048-914E-9901-A2032154BA9D}" yWindow="2800"/>
+    <workbookView windowHeight="17440" windowWidth="28040" xWindow="11580" xr2:uid="{EC5A81AB-0C03-7C45-911F-2BEA6CC0EC9C}" yWindow="1800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -56,19 +56,37 @@
     <t>D001</t>
   </si>
   <si>
+    <t>AVAILABLE</t>
+  </si>
+  <si>
     <t>D002</t>
   </si>
   <si>
-    <t>AVAILABLE</t>
-  </si>
-  <si>
-    <t>10:00 AM</t>
-  </si>
-  <si>
-    <t>12:00 PM</t>
+    <t>12:00 pm</t>
+  </si>
+  <si>
+    <t>01:00 pm</t>
   </si>
   <si>
     <t>BUSY</t>
+  </si>
+  <si>
+    <t>02:00 pm</t>
+  </si>
+  <si>
+    <t>03:00 pm</t>
+  </si>
+  <si>
+    <t>04:00 pm</t>
+  </si>
+  <si>
+    <t>05:00 pm</t>
+  </si>
+  <si>
+    <t>06:00 pm</t>
+  </si>
+  <si>
+    <t>07:00 pm</t>
   </si>
 </sst>
 </file>
@@ -78,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/MM/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,11 +105,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -130,11 +153,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="18" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -469,94 +501,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C808D-9F34-F242-8D47-07932BD88B7B}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFAD5FD-C648-5544-8970-A22DD9CDDA3A}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="31.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.6640625" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>45595</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.375</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45595</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45596</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>45595</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="n" s="4">
-        <v>45593.0</v>
+      <c r="B5" s="5" t="n">
+        <v>45599.0</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -566,6 +593,142 @@
       </c>
       <c r="E5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>45599.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>45600.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>45600.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>45601.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>45601.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>45599.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="12" t="n">
+        <v>45599.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="n" s="13">
+        <v>45599.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>